<commit_message>
inserção das métricas de qualidade do sonarqube
</commit_message>
<xml_diff>
--- a/resultados parciais.xlsx
+++ b/resultados parciais.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>Metricas Coletadas</t>
   </si>
@@ -58,6 +58,24 @@
     <t xml:space="preserve">Reputação </t>
   </si>
   <si>
+    <t>vulnerabilidades</t>
+  </si>
+  <si>
+    <t>blocos duplicados</t>
+  </si>
+  <si>
+    <t>code smells</t>
+  </si>
+  <si>
+    <t>lihas duplicadas</t>
+  </si>
+  <si>
+    <t>bugs</t>
+  </si>
+  <si>
+    <t>Percentual de cobertura de testes</t>
+  </si>
+  <si>
     <t>jwd-ali</t>
   </si>
   <si>
@@ -176,6 +194,12 @@
   </si>
   <si>
     <t>Escala da reputação</t>
+  </si>
+  <si>
+    <t>indice de confiança de qualidade do soarqube</t>
+  </si>
+  <si>
+    <t>Escala de cobertura de testes</t>
   </si>
   <si>
     <t>Score Geral</t>
@@ -242,7 +266,51 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,7 +325,77 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,120 +408,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -412,19 +436,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,163 +616,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,13 +658,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,7 +677,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,6 +706,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -689,30 +728,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -731,6 +746,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -740,146 +764,146 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -901,6 +925,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1230,10 +1263,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:N26"/>
+  <dimension ref="B1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6666666666667" defaultRowHeight="14.4"/>
@@ -1262,7 +1295,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" ht="41.4" spans="2:14">
+    <row r="3" ht="55.2" spans="2:20">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1302,31 +1335,49 @@
       <c r="N3" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="O3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:20">
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4">
         <v>1780632</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
@@ -1335,7 +1386,7 @@
         <v>1.6</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M4" s="5">
         <v>1.67</v>
@@ -1343,40 +1394,58 @@
       <c r="N4" s="5">
         <v>5414</v>
       </c>
+      <c r="O4" s="9">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0</v>
+      </c>
+      <c r="R4" s="9">
+        <v>0</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0</v>
+      </c>
+      <c r="T4" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:20">
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4">
         <v>5783700</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K5" s="5">
         <v>3.25</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="M5" s="5">
         <v>1.12</v>
@@ -1384,40 +1453,60 @@
       <c r="N5" s="5">
         <v>2872</v>
       </c>
+      <c r="O5" s="9">
+        <v>0</v>
+      </c>
+      <c r="P5" s="9">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="9">
+        <f>198+36</f>
+        <v>234</v>
+      </c>
+      <c r="R5" s="9">
+        <f>639+39</f>
+        <v>678</v>
+      </c>
+      <c r="S5" s="9">
+        <v>38</v>
+      </c>
+      <c r="T5" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:20">
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4">
         <v>355715</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E6" s="5">
         <v>35</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="K6" s="5">
         <v>0.22</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="M6" s="5">
         <v>1.15</v>
@@ -1425,31 +1514,49 @@
       <c r="N6" s="5">
         <v>4123</v>
       </c>
+      <c r="O6" s="9">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>165</v>
+      </c>
+      <c r="R6" s="9">
+        <v>5338</v>
+      </c>
+      <c r="S6" s="9">
+        <v>10</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:20">
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4">
         <v>2312051</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5">
         <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J7" s="5">
         <v>0</v>
@@ -1458,7 +1565,7 @@
         <v>2.31</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="M7" s="5">
         <v>0.08</v>
@@ -1466,10 +1573,28 @@
       <c r="N7" s="5">
         <v>3698</v>
       </c>
+      <c r="O7" s="9">
+        <v>0</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0</v>
+      </c>
+      <c r="R7" s="9">
+        <v>0</v>
+      </c>
+      <c r="S7" s="9">
+        <v>0</v>
+      </c>
+      <c r="T7" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:20">
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C8" s="4">
         <v>2576254</v>
@@ -1484,37 +1609,55 @@
         <v>0</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K8" s="5">
         <v>1.08</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="M8" s="5">
         <v>0.53</v>
       </c>
       <c r="N8" s="5">
         <v>4540</v>
+      </c>
+      <c r="O8" s="9">
+        <v>1</v>
+      </c>
+      <c r="P8" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>10</v>
+      </c>
+      <c r="R8" s="9">
+        <v>84</v>
+      </c>
+      <c r="S8" s="9">
+        <v>9</v>
+      </c>
+      <c r="T8" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" ht="69" spans="2:11">
+    <row r="12" ht="69" spans="2:13">
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1522,33 +1665,39 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:13">
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4">
         <v>1780632</v>
@@ -1577,10 +1726,16 @@
       <c r="K13" s="6">
         <v>4</v>
       </c>
+      <c r="L13" s="10">
+        <v>1</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:13">
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C14" s="4">
         <v>5783700</v>
@@ -1609,10 +1764,16 @@
       <c r="K14" s="6">
         <v>3</v>
       </c>
+      <c r="L14" s="10">
+        <v>3</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:13">
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4">
         <v>355715</v>
@@ -1641,10 +1802,16 @@
       <c r="K15" s="6">
         <v>4</v>
       </c>
+      <c r="L15" s="10">
+        <v>3</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:13">
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C16" s="4">
         <v>2312051</v>
@@ -1673,10 +1840,16 @@
       <c r="K16" s="6">
         <v>4</v>
       </c>
+      <c r="L16" s="10">
+        <v>1</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:13">
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4">
         <v>2576254</v>
@@ -1704,15 +1877,21 @@
       </c>
       <c r="K17" s="6">
         <v>4</v>
+      </c>
+      <c r="L17" s="10">
+        <v>3</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="I20" s="2"/>
     </row>
@@ -1724,55 +1903,55 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" ht="67.2" spans="2:10">
       <c r="B22" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C22" s="4">
         <v>5783700</v>
       </c>
       <c r="D22" s="8">
-        <f>AVERAGE(D14:K14)</f>
-        <v>2.875</v>
+        <f>AVERAGE(D14:M14)</f>
+        <v>2.6</v>
       </c>
       <c r="E22" s="8">
         <v>1</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J22" s="10">
+        <v>68</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C23" s="4">
         <v>2312051</v>
       </c>
       <c r="D23" s="8">
-        <f>AVERAGE(D16:K16)</f>
-        <v>2.625</v>
+        <f>AVERAGE(D16:M16)</f>
+        <v>2.2</v>
       </c>
       <c r="E23" s="8">
         <v>2</v>
@@ -1780,14 +1959,14 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4">
-        <v>2576254</v>
+        <v>355715</v>
       </c>
       <c r="D24" s="8">
-        <f>AVERAGE(D17:K17)</f>
-        <v>1.75</v>
+        <f>AVERAGE(D15:M15)</f>
+        <v>1.8</v>
       </c>
       <c r="E24" s="8">
         <v>3</v>
@@ -1795,14 +1974,14 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C25" s="4">
-        <v>355715</v>
+        <v>2576254</v>
       </c>
       <c r="D25" s="8">
-        <f>AVERAGE(D15:K15)</f>
-        <v>1.875</v>
+        <f>AVERAGE(D17:M17)</f>
+        <v>1.7</v>
       </c>
       <c r="E25" s="8">
         <v>4</v>
@@ -1810,14 +1989,14 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4">
         <v>1780632</v>
       </c>
       <c r="D26" s="8">
-        <f>AVERAGE(D13:K13)</f>
-        <v>1.625</v>
+        <f>AVERAGE(D13:M13)</f>
+        <v>1.4</v>
       </c>
       <c r="E26" s="8">
         <v>5</v>

</xml_diff>